<commit_message>
WIP - Donor Focus analysis
</commit_message>
<xml_diff>
--- a/data-raw/unhcr_2022/iati_humanitarian_scope.xlsx
+++ b/data-raw/unhcr_2022/iati_humanitarian_scope.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H227"/>
+  <dimension ref="A1:G227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -385,15 +385,10 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>humanitarian_scope_pct</t>
+          <t>humanitarian_scope_desc_eng</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>humanitarian_scope_desc_eng</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>humanitarian_scope_desc_fr</t>
         </is>
@@ -425,12 +420,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -462,12 +457,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -499,12 +494,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -536,12 +531,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -573,12 +568,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -610,12 +605,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -647,12 +642,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -684,12 +679,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -721,12 +716,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -758,12 +753,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -795,7 +790,7 @@
           <t>RREG22</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>Refugee and Migrant Response Plan for Venezuela 2022 (RMRP)</t>
         </is>
@@ -827,12 +822,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -864,12 +859,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -901,7 +896,7 @@
           <t>HCOL22</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>Colombia Plan de Respuesta Humanitario 2022</t>
         </is>
@@ -933,7 +928,7 @@
           <t>RREG22</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Refugee and Migrant Response Plan for Venezuela 2022 (RMRP)</t>
         </is>
@@ -965,12 +960,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1002,12 +997,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1039,7 +1034,7 @@
           <t>RREG22</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>Refugee and Migrant Response Plan for Venezuela 2022 (RMRP)</t>
         </is>
@@ -1071,12 +1066,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1108,12 +1103,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1140,7 +1135,7 @@
           <t>HHND2122</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>Honduras Plan de Respuesta Humanitario 2021</t>
         </is>
@@ -1172,7 +1167,7 @@
           <t>HHND22</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>Honduras Plan de Respuesta Humanitario 2022</t>
         </is>
@@ -1204,12 +1199,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1241,7 +1236,7 @@
           <t>RREG22</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>Refugee and Migrant Response Plan for Venezuela 2022 (RMRP)</t>
         </is>
@@ -1273,12 +1268,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1310,12 +1305,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G27" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1347,7 +1342,7 @@
           <t>RREG22</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>Refugee and Migrant Response Plan for Venezuela 2022 (RMRP)</t>
         </is>
@@ -1379,12 +1374,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G29" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1416,12 +1411,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1453,7 +1448,7 @@
           <t>RREG22</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>Refugee and Migrant Response Plan for Venezuela 2022 (RMRP)</t>
         </is>
@@ -1485,12 +1480,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G32" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1517,7 +1512,7 @@
           <t>HSLV2122</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>El Salvador Plan de Respuesta Humanitario 2021</t>
         </is>
@@ -1549,12 +1544,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G34" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1586,12 +1581,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G35" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1623,7 +1618,7 @@
           <t>HVEN22</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>Venezuela Plan de Respuesta Humanitario 2022</t>
         </is>
@@ -1655,12 +1650,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G37" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1687,7 +1682,7 @@
           <t>HAFG22</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>Afghanistan Humanitarian Response Plan 2022</t>
         </is>
@@ -1719,7 +1714,7 @@
           <t>RAFG22</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>Afghanistan Regional Refugee Response Plan 2022</t>
         </is>
@@ -1751,12 +1746,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G40" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1788,12 +1783,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G41" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1825,7 +1820,7 @@
           <t>RBGD22</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>Bangladesh: Rohingya Humanitarian Crisis Joint Response Plan 2022</t>
         </is>
@@ -1857,12 +1852,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G43" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1894,12 +1889,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G44" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1931,12 +1926,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G45" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -1968,12 +1963,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G46" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2005,7 +2000,7 @@
           <t>RAFG22</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>Afghanistan Regional Refugee Response Plan 2022</t>
         </is>
@@ -2037,12 +2032,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G48" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2074,12 +2069,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G49" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2111,7 +2106,7 @@
           <t>RAFG22</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>Afghanistan Regional Refugee Response Plan 2022</t>
         </is>
@@ -2143,12 +2138,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G51" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2180,12 +2175,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G52" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2217,12 +2212,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G53" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2254,7 +2249,7 @@
           <t>HMMR22</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="F54" t="inlineStr">
         <is>
           <t>Myanmar Humanitarian Response Plan 2022</t>
         </is>
@@ -2286,12 +2281,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G55" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2323,12 +2318,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G56" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2355,7 +2350,7 @@
           <t>FL-2022-000270-PAK</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>Pakistan: Flood</t>
         </is>
@@ -2387,12 +2382,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G58" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2424,7 +2419,7 @@
           <t>OPAK2223</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr">
+      <c r="F59" t="inlineStr">
         <is>
           <t>Pakistan Floods Response Plan 2022</t>
         </is>
@@ -2456,7 +2451,7 @@
           <t>PAKISTAN-FLOOD-RESPONSE-2022</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="F60" t="inlineStr">
         <is>
           <t>Pakistan Flood Response Supplementary Appeal</t>
         </is>
@@ -2488,7 +2483,7 @@
           <t>PAKISTAN-FLOOD-RESPONSE-2023</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="F61" t="inlineStr">
         <is>
           <t>Pakistan Flood Response, UNHCR Supplementary Appeal, September 2022-December 2023</t>
         </is>
@@ -2520,7 +2515,7 @@
           <t>RAFG22</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="F62" t="inlineStr">
         <is>
           <t>Afghanistan Regional Refugee Response Plan 2022</t>
         </is>
@@ -2552,12 +2547,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G63" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2589,12 +2584,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G64" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2626,12 +2621,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G65" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2663,12 +2658,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G66" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2700,12 +2695,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G67" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2737,7 +2732,7 @@
           <t>RAFG22</t>
         </is>
       </c>
-      <c r="G68" t="inlineStr">
+      <c r="F68" t="inlineStr">
         <is>
           <t>Afghanistan Regional Refugee Response Plan 2022</t>
         </is>
@@ -2769,12 +2764,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G69" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2801,7 +2796,7 @@
           <t>HBDI22</t>
         </is>
       </c>
-      <c r="G70" t="inlineStr">
+      <c r="F70" t="inlineStr">
         <is>
           <t>Burundi Humanitarian Response Plan 2022</t>
         </is>
@@ -2833,7 +2828,7 @@
           <t>RDRCRRP22</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="F71" t="inlineStr">
         <is>
           <t>Democratic Republic of Congo Regional Refugee Response Plan 2022</t>
         </is>
@@ -2865,12 +2860,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G72" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2902,12 +2897,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G73" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2939,12 +2934,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G74" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -2976,7 +2971,7 @@
           <t>HETH22</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr">
+      <c r="F75" t="inlineStr">
         <is>
           <t>Ethiopia Humanitarian Response Plan 2022</t>
         </is>
@@ -3008,7 +3003,7 @@
           <t>RSSDRRP22</t>
         </is>
       </c>
-      <c r="G76" t="inlineStr">
+      <c r="F76" t="inlineStr">
         <is>
           <t>South Sudan Regional Refugee Response Plan 2022</t>
         </is>
@@ -3040,12 +3035,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G77" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3077,7 +3072,7 @@
           <t>RSSDRRP22</t>
         </is>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="F78" t="inlineStr">
         <is>
           <t>South Sudan Regional Refugee Response Plan 2022</t>
         </is>
@@ -3109,12 +3104,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G79" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3146,12 +3141,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G80" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3183,12 +3178,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G81" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3220,12 +3215,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G82" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3257,7 +3252,7 @@
           <t>RDRCRRP22</t>
         </is>
       </c>
-      <c r="G83" t="inlineStr">
+      <c r="F83" t="inlineStr">
         <is>
           <t>Democratic Republic of Congo Regional Refugee Response Plan 2022</t>
         </is>
@@ -3289,7 +3284,7 @@
           <t>FL-2022-000277-SDN</t>
         </is>
       </c>
-      <c r="G84" t="inlineStr">
+      <c r="F84" t="inlineStr">
         <is>
           <t>Sudan: Floods</t>
         </is>
@@ -3321,12 +3316,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G85" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3358,7 +3353,7 @@
           <t>HSDN22</t>
         </is>
       </c>
-      <c r="G86" t="inlineStr">
+      <c r="F86" t="inlineStr">
         <is>
           <t>Sudan Humanitarian Response Plan 2022</t>
         </is>
@@ -3390,7 +3385,7 @@
           <t>RSSDRRP22</t>
         </is>
       </c>
-      <c r="G87" t="inlineStr">
+      <c r="F87" t="inlineStr">
         <is>
           <t>South Sudan Regional Refugee Response Plan 2022</t>
         </is>
@@ -3422,7 +3417,7 @@
           <t>SDN-COUNTRY-RRP-2022</t>
         </is>
       </c>
-      <c r="G88" t="inlineStr">
+      <c r="F88" t="inlineStr">
         <is>
           <t>Sudan - Country Refugee Response Plan - 2022</t>
         </is>
@@ -3454,12 +3449,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G89" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3491,7 +3486,7 @@
           <t>HSOM22</t>
         </is>
       </c>
-      <c r="G90" t="inlineStr">
+      <c r="F90" t="inlineStr">
         <is>
           <t>Somalia Humanitarian Response Plan 2022</t>
         </is>
@@ -3523,12 +3518,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G91" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3560,7 +3555,7 @@
           <t>HSSD22</t>
         </is>
       </c>
-      <c r="G92" t="inlineStr">
+      <c r="F92" t="inlineStr">
         <is>
           <t>South Sudan Humanitarian Response Plan 2022</t>
         </is>
@@ -3592,12 +3587,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G93" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3629,7 +3624,7 @@
           <t>RDRCRRP22</t>
         </is>
       </c>
-      <c r="G94" t="inlineStr">
+      <c r="F94" t="inlineStr">
         <is>
           <t>Democratic Republic of Congo Regional Refugee Response Plan 2022</t>
         </is>
@@ -3656,7 +3651,7 @@
           <t>CE-2022-000195-UGA</t>
         </is>
       </c>
-      <c r="G95" t="inlineStr">
+      <c r="F95" t="inlineStr">
         <is>
           <t>Uganda: Complex Emergency</t>
         </is>
@@ -3688,12 +3683,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G96" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3725,7 +3720,7 @@
           <t>RDRCRRP22</t>
         </is>
       </c>
-      <c r="G97" t="inlineStr">
+      <c r="F97" t="inlineStr">
         <is>
           <t>Democratic Republic of Congo Regional Refugee Response Plan 2022</t>
         </is>
@@ -3757,7 +3752,7 @@
           <t>RSSDRRP22</t>
         </is>
       </c>
-      <c r="G98" t="inlineStr">
+      <c r="F98" t="inlineStr">
         <is>
           <t>South Sudan Regional Refugee Response Plan 2022</t>
         </is>
@@ -3789,7 +3784,7 @@
           <t>UGANDA-COUNTRY-RRP-2022</t>
         </is>
       </c>
-      <c r="G99" t="inlineStr">
+      <c r="F99" t="inlineStr">
         <is>
           <t>Uganda Country Refugee Response Plan - Emergency Appeal - April-June 2022</t>
         </is>
@@ -3821,7 +3816,7 @@
           <t>UGANDA-COUNTRY-RRP-2022-APR-DEC</t>
         </is>
       </c>
-      <c r="G100" t="inlineStr">
+      <c r="F100" t="inlineStr">
         <is>
           <t>Uganda: 2022 Revised Refugee Response Plan | Emergency Appeal</t>
         </is>
@@ -3853,12 +3848,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G101" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3890,12 +3885,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G102" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3927,12 +3922,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G103" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -3964,12 +3959,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G104" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4001,12 +3996,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G105" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4038,12 +4033,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G106" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4075,12 +4070,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G107" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4112,12 +4107,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G108" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4149,12 +4144,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G109" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4186,12 +4181,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G110" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4223,12 +4218,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G111" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4260,12 +4255,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G112" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4297,12 +4292,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G113" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4334,12 +4329,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G114" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H114" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4371,12 +4366,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G115" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H115" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4403,7 +4398,7 @@
           <t>RUKRN22</t>
         </is>
       </c>
-      <c r="G116" t="inlineStr">
+      <c r="F116" t="inlineStr">
         <is>
           <t>Ukraine Regional Refugee Response Plan 2022 (March - August 2022)</t>
         </is>
@@ -4435,7 +4430,7 @@
           <t>UKRAINE-SITUATION-2022</t>
         </is>
       </c>
-      <c r="G117" t="inlineStr">
+      <c r="F117" t="inlineStr">
         <is>
           <t>Ukraine Situation - Supplementary Appeal 2022</t>
         </is>
@@ -4467,7 +4462,7 @@
           <t>UKRAINE-SITUATION-2022-REVISED</t>
         </is>
       </c>
-      <c r="G118" t="inlineStr">
+      <c r="F118" t="inlineStr">
         <is>
           <t>Ukraine Situation - Revised Supplementary Appeal 2022</t>
         </is>
@@ -4499,12 +4494,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G119" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H119" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4536,12 +4531,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G120" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H120" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4573,12 +4568,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G121" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H121" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4610,12 +4605,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G122" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H122" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4647,12 +4642,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G123" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H123" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4684,12 +4679,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G124" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H124" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4721,12 +4716,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G125" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H125" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4753,7 +4748,7 @@
           <t>RUKRN22</t>
         </is>
       </c>
-      <c r="G126" t="inlineStr">
+      <c r="F126" t="inlineStr">
         <is>
           <t>Ukraine Regional Refugee Response Plan 2022 (March - August 2022)</t>
         </is>
@@ -4785,7 +4780,7 @@
           <t>UKRAINE-SITUATION-2022</t>
         </is>
       </c>
-      <c r="G127" t="inlineStr">
+      <c r="F127" t="inlineStr">
         <is>
           <t>Ukraine Situation - Supplementary Appeal 2022</t>
         </is>
@@ -4817,7 +4812,7 @@
           <t>UKRAINE-SITUATION-2022-REVISED</t>
         </is>
       </c>
-      <c r="G128" t="inlineStr">
+      <c r="F128" t="inlineStr">
         <is>
           <t>Ukraine Situation - Revised Supplementary Appeal 2022</t>
         </is>
@@ -4849,12 +4844,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G129" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H129" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4886,12 +4881,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G130" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H130" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -4918,7 +4913,7 @@
           <t>RUKRN22</t>
         </is>
       </c>
-      <c r="G131" t="inlineStr">
+      <c r="F131" t="inlineStr">
         <is>
           <t>Ukraine Regional Refugee Response Plan 2022 (March - August 2022)</t>
         </is>
@@ -4950,7 +4945,7 @@
           <t>UKRAINE-SITUATION-2022</t>
         </is>
       </c>
-      <c r="G132" t="inlineStr">
+      <c r="F132" t="inlineStr">
         <is>
           <t>Ukraine Situation - Supplementary Appeal 2022</t>
         </is>
@@ -4982,7 +4977,7 @@
           <t>UKRAINE-SITUATION-2022-REVISED</t>
         </is>
       </c>
-      <c r="G133" t="inlineStr">
+      <c r="F133" t="inlineStr">
         <is>
           <t>Ukraine Situation - Revised Supplementary Appeal 2022</t>
         </is>
@@ -5014,12 +5009,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G134" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H134" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5046,7 +5041,7 @@
           <t>RUKRN22</t>
         </is>
       </c>
-      <c r="G135" t="inlineStr">
+      <c r="F135" t="inlineStr">
         <is>
           <t>Ukraine Regional Refugee Response Plan 2022 (March - August 2022)</t>
         </is>
@@ -5078,7 +5073,7 @@
           <t>UKRAINE-SITUATION-2022</t>
         </is>
       </c>
-      <c r="G136" t="inlineStr">
+      <c r="F136" t="inlineStr">
         <is>
           <t>Ukraine Situation - Supplementary Appeal 2022</t>
         </is>
@@ -5110,7 +5105,7 @@
           <t>UKRAINE-SITUATION-2022-REVISED</t>
         </is>
       </c>
-      <c r="G137" t="inlineStr">
+      <c r="F137" t="inlineStr">
         <is>
           <t>Ukraine Situation - Revised Supplementary Appeal 2022</t>
         </is>
@@ -5142,12 +5137,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G138" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H138" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5179,12 +5174,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G139" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H139" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5216,12 +5211,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G140" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H140" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5253,12 +5248,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G141" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H141" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5290,7 +5285,7 @@
           <t>RSYR22</t>
         </is>
       </c>
-      <c r="G142" t="inlineStr">
+      <c r="F142" t="inlineStr">
         <is>
           <t>Syria Refugee Response and Resilience Plan (3RP) 2022</t>
         </is>
@@ -5322,7 +5317,7 @@
           <t>SYRIA-3RP-REGIONAL-STRATEGIC-OVERVIEW-2021-2022</t>
         </is>
       </c>
-      <c r="G143" t="inlineStr">
+      <c r="F143" t="inlineStr">
         <is>
           <t>Syria 3RP Regional Strategic Overview 2021-2022</t>
         </is>
@@ -5349,7 +5344,7 @@
           <t>FUKR22</t>
         </is>
       </c>
-      <c r="G144" t="inlineStr">
+      <c r="F144" t="inlineStr">
         <is>
           <t>Ukraine Flash Appeal 2022</t>
         </is>
@@ -5381,12 +5376,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G145" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H145" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5413,7 +5408,7 @@
           <t>HUKR22</t>
         </is>
       </c>
-      <c r="G146" t="inlineStr">
+      <c r="F146" t="inlineStr">
         <is>
           <t>Ukraine Humanitarian Response Plan 2022</t>
         </is>
@@ -5445,7 +5440,7 @@
           <t>UKRAINE-SITUATION-2022</t>
         </is>
       </c>
-      <c r="G147" t="inlineStr">
+      <c r="F147" t="inlineStr">
         <is>
           <t>Ukraine Situation - Supplementary Appeal 2022</t>
         </is>
@@ -5477,7 +5472,7 @@
           <t>UKRAINE-SITUATION-2022-REVISED</t>
         </is>
       </c>
-      <c r="G148" t="inlineStr">
+      <c r="F148" t="inlineStr">
         <is>
           <t>Ukraine Situation - Revised Supplementary Appeal 2022</t>
         </is>
@@ -5509,12 +5504,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G149" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H149" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5546,12 +5541,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G150" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H150" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5583,12 +5578,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G151" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H151" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5620,12 +5615,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G152" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H152" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5657,12 +5652,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G153" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H153" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5694,7 +5689,7 @@
           <t>RSYR22</t>
         </is>
       </c>
-      <c r="G154" t="inlineStr">
+      <c r="F154" t="inlineStr">
         <is>
           <t>Syria Refugee Response and Resilience Plan (3RP) 2022</t>
         </is>
@@ -5726,7 +5721,7 @@
           <t>SYRIA-3RP-REGIONAL-STRATEGIC-OVERVIEW-2021-2022</t>
         </is>
       </c>
-      <c r="G155" t="inlineStr">
+      <c r="F155" t="inlineStr">
         <is>
           <t>Syria 3RP Regional Strategic Overview 2021-2022</t>
         </is>
@@ -5758,12 +5753,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G156" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H156" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5795,12 +5790,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G157" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H157" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5832,7 +5827,7 @@
           <t>HIRQ22</t>
         </is>
       </c>
-      <c r="G158" t="inlineStr">
+      <c r="F158" t="inlineStr">
         <is>
           <t>Iraq Humanitarian Response Plan 2022</t>
         </is>
@@ -5864,7 +5859,7 @@
           <t>RSYR22</t>
         </is>
       </c>
-      <c r="G159" t="inlineStr">
+      <c r="F159" t="inlineStr">
         <is>
           <t>Syria Refugee Response and Resilience Plan (3RP) 2022</t>
         </is>
@@ -5896,7 +5891,7 @@
           <t>SYRIA-3RP-REGIONAL-STRATEGIC-OVERVIEW-2021-2022</t>
         </is>
       </c>
-      <c r="G160" t="inlineStr">
+      <c r="F160" t="inlineStr">
         <is>
           <t>Syria 3RP Regional Strategic Overview 2021-2022</t>
         </is>
@@ -5928,12 +5923,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G161" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H161" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -5965,12 +5960,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G162" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H162" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6002,7 +5997,7 @@
           <t>RSYR22</t>
         </is>
       </c>
-      <c r="G163" t="inlineStr">
+      <c r="F163" t="inlineStr">
         <is>
           <t>Syria Refugee Response and Resilience Plan (3RP) 2022</t>
         </is>
@@ -6034,7 +6029,7 @@
           <t>SYRIA-3RP-REGIONAL-STRATEGIC-OVERVIEW-2021-2022</t>
         </is>
       </c>
-      <c r="G164" t="inlineStr">
+      <c r="F164" t="inlineStr">
         <is>
           <t>Syria 3RP Regional Strategic Overview 2021-2022</t>
         </is>
@@ -6066,12 +6061,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G165" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H165" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6098,7 +6093,7 @@
           <t>OLBN2122</t>
         </is>
       </c>
-      <c r="G166" t="inlineStr">
+      <c r="F166" t="inlineStr">
         <is>
           <t>Lebanon Emergency Response Plan 2021</t>
         </is>
@@ -6130,7 +6125,7 @@
           <t>RSYR22</t>
         </is>
       </c>
-      <c r="G167" t="inlineStr">
+      <c r="F167" t="inlineStr">
         <is>
           <t>Syria Refugee Response and Resilience Plan (3RP) 2022</t>
         </is>
@@ -6162,7 +6157,7 @@
           <t>SYRIA-3RP-REGIONAL-STRATEGIC-OVERVIEW-2021-2022</t>
         </is>
       </c>
-      <c r="G168" t="inlineStr">
+      <c r="F168" t="inlineStr">
         <is>
           <t>Syria 3RP Regional Strategic Overview 2021-2022</t>
         </is>
@@ -6194,12 +6189,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G169" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H169" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6231,7 +6226,7 @@
           <t>HLBY22</t>
         </is>
       </c>
-      <c r="G170" t="inlineStr">
+      <c r="F170" t="inlineStr">
         <is>
           <t>Libya Humanitarian Response Plan 2022</t>
         </is>
@@ -6263,12 +6258,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G171" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H171" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6300,12 +6295,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G172" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H172" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6337,12 +6332,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G173" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H173" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6374,12 +6369,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G174" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H174" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6411,12 +6406,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G175" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H175" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6448,12 +6443,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G176" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H176" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6485,12 +6480,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G177" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H177" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6522,7 +6517,7 @@
           <t>HSYR22</t>
         </is>
       </c>
-      <c r="G178" t="inlineStr">
+      <c r="F178" t="inlineStr">
         <is>
           <t>Syria Humanitarian Response Plan 2022 - 2023</t>
         </is>
@@ -6554,7 +6549,7 @@
           <t>RSYR22</t>
         </is>
       </c>
-      <c r="G179" t="inlineStr">
+      <c r="F179" t="inlineStr">
         <is>
           <t>Syria Refugee Response and Resilience Plan (3RP) 2022</t>
         </is>
@@ -6586,7 +6581,7 @@
           <t>SYRIA-3RP-REGIONAL-STRATEGIC-OVERVIEW-2021-2022</t>
         </is>
       </c>
-      <c r="G180" t="inlineStr">
+      <c r="F180" t="inlineStr">
         <is>
           <t>Syria 3RP Regional Strategic Overview 2021-2022</t>
         </is>
@@ -6618,12 +6613,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G181" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H181" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6655,12 +6650,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G182" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H182" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6692,7 +6687,7 @@
           <t>HYEM22</t>
         </is>
       </c>
-      <c r="G183" t="inlineStr">
+      <c r="F183" t="inlineStr">
         <is>
           <t>Yemen Humanitarian Response Plan 2022</t>
         </is>
@@ -6724,12 +6719,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G184" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H184" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6761,7 +6756,7 @@
           <t>RDRCRRP22</t>
         </is>
       </c>
-      <c r="G185" t="inlineStr">
+      <c r="F185" t="inlineStr">
         <is>
           <t>Democratic Republic of Congo Regional Refugee Response Plan 2022</t>
         </is>
@@ -6793,7 +6788,7 @@
           <t>CE-2022-000235-COD</t>
         </is>
       </c>
-      <c r="G186" t="inlineStr">
+      <c r="F186" t="inlineStr">
         <is>
           <t>Democratic Republic of the Congo: Complex Emergency</t>
         </is>
@@ -6825,12 +6820,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G187" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H187" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6862,7 +6857,7 @@
           <t>HCOD22</t>
         </is>
       </c>
-      <c r="G188" t="inlineStr">
+      <c r="F188" t="inlineStr">
         <is>
           <t>République Démocratique du Congo Plan de Réponse Humanitaire 2022</t>
         </is>
@@ -6894,7 +6889,7 @@
           <t>RSSDRRP22</t>
         </is>
       </c>
-      <c r="G189" t="inlineStr">
+      <c r="F189" t="inlineStr">
         <is>
           <t>South Sudan Regional Refugee Response Plan 2022</t>
         </is>
@@ -6926,7 +6921,7 @@
           <t>CE-2022-000317-COG</t>
         </is>
       </c>
-      <c r="G190" t="inlineStr">
+      <c r="F190" t="inlineStr">
         <is>
           <t>Republic of the Congo: Complex Emergency</t>
         </is>
@@ -6958,12 +6953,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G191" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H191" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -6995,7 +6990,7 @@
           <t>RDRCRRP22</t>
         </is>
       </c>
-      <c r="G192" t="inlineStr">
+      <c r="F192" t="inlineStr">
         <is>
           <t>Democratic Republic of Congo Regional Refugee Response Plan 2022</t>
         </is>
@@ -7027,7 +7022,7 @@
           <t>FMOZ22</t>
         </is>
       </c>
-      <c r="G193" t="inlineStr">
+      <c r="F193" t="inlineStr">
         <is>
           <t>Mozambique Gombe Emergency Response Plan 2022</t>
         </is>
@@ -7059,12 +7054,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G194" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H194" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7096,7 +7091,7 @@
           <t>HMOZ22</t>
         </is>
       </c>
-      <c r="G195" t="inlineStr">
+      <c r="F195" t="inlineStr">
         <is>
           <t>Mozambique Humanitarian Response Plan 2022</t>
         </is>
@@ -7123,7 +7118,7 @@
           <t>TC-2022-000184-MOZ</t>
         </is>
       </c>
-      <c r="G196" t="inlineStr">
+      <c r="F196" t="inlineStr">
         <is>
           <t>Mozambique: Tropical Cyclone</t>
         </is>
@@ -7155,12 +7150,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G197" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H197" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7192,12 +7187,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G198" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H198" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7229,12 +7224,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G199" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H199" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7266,12 +7261,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G200" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H200" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7303,12 +7298,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G201" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H201" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7340,7 +7335,7 @@
           <t>RDRCRRP22</t>
         </is>
       </c>
-      <c r="G202" t="inlineStr">
+      <c r="F202" t="inlineStr">
         <is>
           <t>Democratic Republic of Congo Regional Refugee Response Plan 2022</t>
         </is>
@@ -7372,12 +7367,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G203" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H203" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7404,7 +7399,7 @@
           <t>CE-2022-000216-BFA</t>
         </is>
       </c>
-      <c r="G204" t="inlineStr">
+      <c r="F204" t="inlineStr">
         <is>
           <t>Burkina Faso: Complex Emergency</t>
         </is>
@@ -7436,12 +7431,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G205" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H205" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7473,7 +7468,7 @@
           <t>HBFA22</t>
         </is>
       </c>
-      <c r="G206" t="inlineStr">
+      <c r="F206" t="inlineStr">
         <is>
           <t>Burkina Faso Plan de Réponse Humanitaire 2022</t>
         </is>
@@ -7505,12 +7500,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G207" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H207" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7542,7 +7537,7 @@
           <t>HCAF22</t>
         </is>
       </c>
-      <c r="G208" t="inlineStr">
+      <c r="F208" t="inlineStr">
         <is>
           <t>République Centrafricaine Plan de Réponse Humanitaire 2022</t>
         </is>
@@ -7574,12 +7569,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G209" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H209" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7611,7 +7606,7 @@
           <t>FAR-NORTH-CAMEROON-SITUATION-2022</t>
         </is>
       </c>
-      <c r="G210" t="inlineStr">
+      <c r="F210" t="inlineStr">
         <is>
           <t>Cameroon and Chad Emergency: Supplementary Appeal January - June 2022</t>
         </is>
@@ -7643,12 +7638,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G211" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H211" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7680,7 +7675,7 @@
           <t>HCMR22</t>
         </is>
       </c>
-      <c r="G212" t="inlineStr">
+      <c r="F212" t="inlineStr">
         <is>
           <t>Cameroon Humanitarian Response Plan 2022</t>
         </is>
@@ -7712,12 +7707,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G213" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H213" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7749,12 +7744,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G214" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H214" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7786,12 +7781,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G215" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H215" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7823,7 +7818,7 @@
           <t>HMLI22</t>
         </is>
       </c>
-      <c r="G216" t="inlineStr">
+      <c r="F216" t="inlineStr">
         <is>
           <t>Mali Plan de Réponse Humanitaire 2022</t>
         </is>
@@ -7855,12 +7850,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G217" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H217" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7892,7 +7887,7 @@
           <t>HNER22</t>
         </is>
       </c>
-      <c r="G218" t="inlineStr">
+      <c r="F218" t="inlineStr">
         <is>
           <t>Niger Plan de Réponse Humanitaire 2022</t>
         </is>
@@ -7924,12 +7919,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G219" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H219" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -7961,7 +7956,7 @@
           <t>HNGA22</t>
         </is>
       </c>
-      <c r="G220" t="inlineStr">
+      <c r="F220" t="inlineStr">
         <is>
           <t>Nigeria Humanitarian Response Plan 2022</t>
         </is>
@@ -7993,12 +7988,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G221" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H221" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -8030,7 +8025,7 @@
           <t>FAR-NORTH-CAMEROON-SITUATION-2022</t>
         </is>
       </c>
-      <c r="G222" t="inlineStr">
+      <c r="F222" t="inlineStr">
         <is>
           <t>Cameroon and Chad Emergency: Supplementary Appeal January - June 2022</t>
         </is>
@@ -8062,12 +8057,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G223" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H223" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -8099,12 +8094,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G224" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H224" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -8136,7 +8131,7 @@
           <t>FAR-NORTH-CAMEROON-SITUATION-2022</t>
         </is>
       </c>
-      <c r="G225" t="inlineStr">
+      <c r="F225" t="inlineStr">
         <is>
           <t>Cameroon and Chad Emergency: Supplementary Appeal January - June 2022</t>
         </is>
@@ -8168,12 +8163,12 @@
           <t>GLOBAL-APPEAL-2022</t>
         </is>
       </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>Global Appeal 2022</t>
+        </is>
+      </c>
       <c r="G226" t="inlineStr">
-        <is>
-          <t>Global Appeal 2022</t>
-        </is>
-      </c>
-      <c r="H226" t="inlineStr">
         <is>
           <t>Appel global 2022</t>
         </is>
@@ -8205,7 +8200,7 @@
           <t>HTCD22</t>
         </is>
       </c>
-      <c r="G227" t="inlineStr">
+      <c r="F227" t="inlineStr">
         <is>
           <t>Tchad Plan de Réponse Humanitaire 2022</t>
         </is>

</xml_diff>